<commit_message>
New Version with updates
This is version 2
</commit_message>
<xml_diff>
--- a/HW3/hw3_9821_fall2023_trees1-q4_karan.xlsx
+++ b/HW3/hw3_9821_fall2023_trees1-q4_karan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karan JESWANI\Desktop\Baruch\Sem1\Numerical Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D81EFBDC-3CB3-4630-9E5F-088E8F7BBFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2C1CB3-3681-4655-91F7-944C0D58036A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="54600" yWindow="-2490" windowWidth="25800" windowHeight="21000" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -311,6 +311,12 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6211,10 +6217,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8502E5C-A055-4A59-83FE-9E98C2648FB0}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6225,23 +6231,23 @@
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:5" s="16" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="16" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>31</v>
       </c>
@@ -6252,13 +6258,13 @@
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>32</v>
       </c>
@@ -6267,7 +6273,7 @@
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
-    <row r="7" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>33</v>
       </c>
@@ -6277,14 +6283,17 @@
       <c r="C7" s="21">
         <v>1</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="23">
         <v>0.27768399999999999</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="23">
         <v>0.27629700000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="23">
+        <v>0.27633799999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>36</v>
       </c>
@@ -6300,8 +6309,11 @@
       <c r="E8" s="22">
         <v>6.3591980000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="22">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>34</v>
       </c>
@@ -6310,18 +6322,18 @@
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="22">
-        <v>0.27629700000000001</v>
+      <c r="B11" s="24">
+        <v>0.27633799999999997</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>

</xml_diff>